<commit_message>
added NA cleanup at end of function and added new egg column to function and template
</commit_message>
<xml_diff>
--- a/inst/extdata/releases_template.xlsx
+++ b/inst/extdata/releases_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bio\LobTag2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DD1B248-85D3-4AAB-A3F9-AA2DD038F8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CCC3F-B568-4F3A-9993-6803DD37020A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SAMPLER</t>
   </si>
@@ -86,12 +86,15 @@
   </si>
   <si>
     <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>EGG_STATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -925,14 +928,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -979,28 +987,34 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified - Non-Classifié&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change to successfull release upload message
</commit_message>
<xml_diff>
--- a/inst/extdata/releases_template.xlsx
+++ b/inst/extdata/releases_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bio\LobTag2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F355A302-E10A-4DC3-9A10-115F35E57CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83C37AB-9407-4E26-BAE1-3B744B4F2048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases_template" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +226,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -932,7 +938,8 @@
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y338" sqref="Y338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1019,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified - Non-Classifié&amp;1#_x000D_</oddHeader>

</xml_diff>